<commit_message>
Number Theory and Array
</commit_message>
<xml_diff>
--- a/SDE Sheet.xlsx
+++ b/SDE Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Src Code\Personal\SDE-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEC2609-690D-4175-BF53-C4D3F9A98E6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF3BF1E-DF15-489B-AE30-CEC3373A7626}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83934561-A72F-4836-B1E7-4EE8C35F9874}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="223">
   <si>
     <t>Matrix</t>
   </si>
@@ -804,6 +804,24 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/merge-intervals/</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-sorted-array/</t>
+  </si>
+  <si>
+    <t>Reservoir Sampling Algorithm</t>
+  </si>
+  <si>
+    <t>Robot Bounded In Circle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/robot-bounded-in-circle/</t>
+  </si>
+  <si>
+    <t>Must revise, new type of solution, Most asked Amazon interview question</t>
   </si>
 </sst>
 </file>
@@ -1115,75 +1133,75 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1500,11 +1518,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EBAEE5-B4E7-4BD5-B694-FD6EEA5E8AC0}">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" zoomScale="44" zoomScaleNormal="94" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1538,14 +1556,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
@@ -1638,14 +1656,14 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
@@ -1756,46 +1774,43 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="56" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="34" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="57" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>18</v>
@@ -1806,154 +1821,157 @@
       <c r="F17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="57" t="s">
+      <c r="G17" s="35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="35" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="57" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="2" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="31"/>
+      <c r="B21" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
-      <c r="B21" s="2" t="s">
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="30"/>
+      <c r="B22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="32"/>
-      <c r="B22" s="2" t="s">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="32"/>
+      <c r="B23" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D23" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="37" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="9"/>
+      <c r="B25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="26"/>
-      <c r="B25" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="26"/>
       <c r="B26" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>18</v>
@@ -1966,318 +1984,336 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="39"/>
-      <c r="B27" s="34" t="s">
+      <c r="A27" s="26"/>
+      <c r="B27" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="41"/>
+      <c r="B28" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C28" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="40"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="2" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="42"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
-      <c r="B29" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="9"/>
+      <c r="B30" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="C30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="29" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="29" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
-      <c r="B31" s="2" t="s">
+    <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="9"/>
+      <c r="B32" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="10"/>
-      <c r="B32" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="29" t="s">
+      <c r="D32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="29" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="44"/>
-      <c r="B33" s="47" t="s">
+    <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="46"/>
+      <c r="B34" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="C33" s="50" t="s">
+      <c r="C34" s="52" t="s">
         <v>184</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="2" t="s">
+      <c r="E34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="45"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="2" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="47"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="45"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="46"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="52"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="53"/>
       <c r="D36" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="48"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="23"/>
-      <c r="B37" s="2" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="23"/>
+      <c r="B38" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C38" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="28"/>
-      <c r="B38" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="28"/>
       <c r="B39" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="28"/>
+      <c r="B40" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C40" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="D40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="25"/>
-      <c r="B40" s="2" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="25"/>
+      <c r="B41" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C41" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="D41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
-      <c r="B41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="9"/>
+      <c r="B43" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="37" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="11"/>
+      <c r="B44" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="9"/>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="9"/>
+      <c r="B46" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="43"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="F46" s="2" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+      <c r="A47" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="45"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
@@ -2288,226 +2324,212 @@
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="11"/>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="11"/>
+      <c r="B52" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="11"/>
-      <c r="B51" s="2" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="11"/>
+      <c r="B53" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="53"/>
-      <c r="B52" s="34" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="55"/>
+      <c r="B54" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C54" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="53"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="2" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="55"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="11"/>
-      <c r="B54" s="2" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="11"/>
+      <c r="B56" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F54" s="2" t="s">
+      <c r="E56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="9"/>
-      <c r="B55" s="2" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="9"/>
+      <c r="B57" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="E57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="9"/>
-      <c r="B56" s="2" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="9"/>
+      <c r="B58" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="D58" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="11"/>
-      <c r="B57" s="2" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="11"/>
+      <c r="B59" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" s="2" t="s">
+      <c r="D59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="38"/>
-      <c r="B58" s="34" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="40"/>
+      <c r="B60" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C60" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="38"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="2" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="40"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" s="2" t="s">
+      <c r="E61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="39"/>
-      <c r="B60" s="34" t="s">
+    <row r="62" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="41"/>
+      <c r="B62" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="C60" s="50" t="s">
+      <c r="C62" s="52" t="s">
         <v>168</v>
-      </c>
-      <c r="D60" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="40"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="54"/>
-      <c r="B62" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="C62" s="50" t="s">
-        <v>171</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>18</v>
@@ -2520,9 +2542,9 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="55"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="52"/>
+      <c r="A63" s="42"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="54"/>
       <c r="D63" s="21" t="s">
         <v>18</v>
       </c>
@@ -2530,158 +2552,158 @@
         <v>4</v>
       </c>
       <c r="F63" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="56"/>
+      <c r="B64" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C64" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="57"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="54"/>
+      <c r="D65" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="39"/>
-      <c r="B64" s="47" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="41"/>
+      <c r="B66" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="C64" s="50" t="s">
+      <c r="C66" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="D64" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="2" t="s">
+      <c r="D66" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" s="40"/>
-      <c r="B65" s="49"/>
-      <c r="C65" s="52"/>
-      <c r="D65" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F65" s="2" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="42"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="54"/>
+      <c r="D67" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="22"/>
-      <c r="B66" s="19" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" s="22"/>
+      <c r="B68" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C68" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="2" t="s">
+      <c r="E68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="17"/>
-      <c r="B67" s="16" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" s="17"/>
+      <c r="B69" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C69" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F67" s="2" t="s">
+      <c r="D69" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="36"/>
-      <c r="B68" s="34" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="38"/>
+      <c r="B70" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C68" s="35" t="s">
+      <c r="C70" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F68" s="2" t="s">
+      <c r="D70" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="36"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="35"/>
-      <c r="D69" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F69" s="2" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" s="38"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="37" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="2"/>
-      <c r="B71" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C71" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="2"/>
-      <c r="B72" s="34"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
-      <c r="B73" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="C73" s="35" t="s">
-        <v>68</v>
+      <c r="B73" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C73" s="37" t="s">
+        <v>63</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>18</v>
@@ -2695,8 +2717,8 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
-      <c r="B74" s="34"/>
-      <c r="C74" s="35"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="37"/>
       <c r="D74" s="2" t="s">
         <v>18</v>
       </c>
@@ -2709,47 +2731,43 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
-      <c r="B75" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>82</v>
+      <c r="B75" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" s="37" t="s">
+        <v>68</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
-      <c r="B76" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>78</v>
-      </c>
+      <c r="B76" s="36"/>
+      <c r="C76" s="37"/>
       <c r="D76" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
-      <c r="B77" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C77" s="35" t="s">
-        <v>84</v>
+      <c r="B77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>18</v>
@@ -2763,25 +2781,29 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="35"/>
+      <c r="B78" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="D78" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
-      <c r="B79" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C79" s="35" t="s">
-        <v>89</v>
+      <c r="B79" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="37" t="s">
+        <v>84</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>18</v>
@@ -2795,8 +2817,8 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
-      <c r="B80" s="34"/>
-      <c r="C80" s="35"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="37"/>
       <c r="D80" s="2" t="s">
         <v>18</v>
       </c>
@@ -2809,171 +2831,171 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
+      <c r="B81" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B82" s="37"/>
+      <c r="A82" s="2"/>
+      <c r="B82" s="36"/>
       <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
+      <c r="D82" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="14"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B84" s="39"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" s="2"/>
+      <c r="B85" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D85" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E85" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F83" s="4"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" s="2"/>
-      <c r="B84" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F84" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="37"/>
+      <c r="F85" s="4"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F86" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E88" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F88" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="37"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
+      <c r="B89" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="37"/>
+      <c r="A90" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" s="39"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="39"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="39"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
-      <c r="B91" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="C91" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" s="2"/>
-      <c r="B92" s="34"/>
-      <c r="C92" s="34"/>
-      <c r="D92" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="A92" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="39"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
-      <c r="B93" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>115</v>
+      <c r="B93" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C93" s="37" t="s">
+        <v>112</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>113</v>
@@ -2981,141 +3003,179 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
-      <c r="B94" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="C94" s="35" t="s">
-        <v>119</v>
-      </c>
+      <c r="B94" s="36"/>
+      <c r="C94" s="36"/>
       <c r="D94" s="2" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="35"/>
+      <c r="B95" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>115</v>
+      </c>
       <c r="D95" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F95" s="13" t="s">
-        <v>121</v>
+      <c r="F95" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A96" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B96" s="37"/>
-      <c r="C96" s="37"/>
-      <c r="D96" s="37"/>
-      <c r="E96" s="37"/>
-      <c r="F96" s="37"/>
+      <c r="A96" s="2"/>
+      <c r="B96" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C96" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
+      <c r="B97" s="36"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B98" s="39"/>
+      <c r="C98" s="39"/>
+      <c r="D98" s="39"/>
+      <c r="E98" s="39"/>
+      <c r="F98" s="39"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F99" s="56" t="s">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F101" s="34" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F102" s="34" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
     <mergeCell ref="A64:A65"/>
+    <mergeCell ref="C64:C65"/>
     <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A96:F96"/>
-    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A98:F98"/>
     <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A84:F84"/>
     <mergeCell ref="B73:B74"/>
     <mergeCell ref="C73:C74"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C54:C55"/>
     <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
     <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A92:F92"/>
+    <mergeCell ref="A87:F87"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{3FB3FA06-DE47-4C2D-AFD7-F5FC45E3D126}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{C4A51F70-7D5B-496B-8FD0-AB7121D9FCE1}"/>
     <hyperlink ref="C9" r:id="rId3" xr:uid="{678D7AA2-36D2-4A02-971F-3FB9391E8E35}"/>
-    <hyperlink ref="C16" r:id="rId4" xr:uid="{2AC6AF52-CC30-4063-833D-09178907C109}"/>
-    <hyperlink ref="C41" r:id="rId5" xr:uid="{6352E065-8925-49FF-AA82-66ED2F9F8651}"/>
-    <hyperlink ref="C17" r:id="rId6" xr:uid="{047C68C0-B7AB-4E77-9D1E-B162BD11A209}"/>
-    <hyperlink ref="C18" r:id="rId7" xr:uid="{1ABD0EDA-F48F-4D2F-B13C-180B398F1FCD}"/>
-    <hyperlink ref="C71" r:id="rId8" xr:uid="{35D2A43C-BF1B-4339-9217-7116005F7034}"/>
-    <hyperlink ref="C73" r:id="rId9" xr:uid="{233456E2-1B15-4448-A669-82C381357683}"/>
-    <hyperlink ref="C86" r:id="rId10" xr:uid="{4A724644-7F2B-4DE6-9141-A1802140FB4A}"/>
-    <hyperlink ref="C83" r:id="rId11" xr:uid="{914A5C5A-20B3-4526-A460-020F9852AFDB}"/>
-    <hyperlink ref="C84" r:id="rId12" xr:uid="{0B2D15B8-18BF-46A5-991E-6E53ADC95851}"/>
-    <hyperlink ref="C24" r:id="rId13" xr:uid="{93A177B9-936F-4ED5-9F32-EB31F0D8F614}"/>
-    <hyperlink ref="C91" r:id="rId14" xr:uid="{9CD2E86C-B1BA-4CC3-9E52-ECA767380715}"/>
-    <hyperlink ref="C93" r:id="rId15" xr:uid="{30EBB8AD-10BE-47B9-BF85-DBCCCE948784}"/>
-    <hyperlink ref="F95" r:id="rId16" xr:uid="{080A2B1B-6640-47F1-9DAB-1F0914BD9938}"/>
-    <hyperlink ref="C50" r:id="rId17" xr:uid="{DD8AB0F8-5B5E-4F6E-A0B4-339B324BDAC3}"/>
+    <hyperlink ref="C17" r:id="rId4" xr:uid="{2AC6AF52-CC30-4063-833D-09178907C109}"/>
+    <hyperlink ref="C42" r:id="rId5" xr:uid="{6352E065-8925-49FF-AA82-66ED2F9F8651}"/>
+    <hyperlink ref="C18" r:id="rId6" xr:uid="{047C68C0-B7AB-4E77-9D1E-B162BD11A209}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{1ABD0EDA-F48F-4D2F-B13C-180B398F1FCD}"/>
+    <hyperlink ref="C73" r:id="rId8" xr:uid="{35D2A43C-BF1B-4339-9217-7116005F7034}"/>
+    <hyperlink ref="C75" r:id="rId9" xr:uid="{233456E2-1B15-4448-A669-82C381357683}"/>
+    <hyperlink ref="C88" r:id="rId10" xr:uid="{4A724644-7F2B-4DE6-9141-A1802140FB4A}"/>
+    <hyperlink ref="C85" r:id="rId11" xr:uid="{914A5C5A-20B3-4526-A460-020F9852AFDB}"/>
+    <hyperlink ref="C86" r:id="rId12" xr:uid="{0B2D15B8-18BF-46A5-991E-6E53ADC95851}"/>
+    <hyperlink ref="C25" r:id="rId13" xr:uid="{93A177B9-936F-4ED5-9F32-EB31F0D8F614}"/>
+    <hyperlink ref="C93" r:id="rId14" xr:uid="{9CD2E86C-B1BA-4CC3-9E52-ECA767380715}"/>
+    <hyperlink ref="C95" r:id="rId15" xr:uid="{30EBB8AD-10BE-47B9-BF85-DBCCCE948784}"/>
+    <hyperlink ref="F97" r:id="rId16" xr:uid="{080A2B1B-6640-47F1-9DAB-1F0914BD9938}"/>
+    <hyperlink ref="C52" r:id="rId17" xr:uid="{DD8AB0F8-5B5E-4F6E-A0B4-339B324BDAC3}"/>
     <hyperlink ref="C7" r:id="rId18" xr:uid="{43B67C49-DC70-412F-B095-E684E07FF196}"/>
-    <hyperlink ref="C60" r:id="rId19" xr:uid="{7FDCAB78-56F5-40D3-8A09-8A8A0E54E05D}"/>
-    <hyperlink ref="F61" r:id="rId20" xr:uid="{F7F3C873-8E94-4212-B22A-52BF75A478D8}"/>
-    <hyperlink ref="C27" r:id="rId21" xr:uid="{F6C15430-DBA9-4DAD-A411-65B1524C625E}"/>
-    <hyperlink ref="G16" r:id="rId22" display="https://leetcode.com/problems/maximum-sum-circular-subarray/" xr:uid="{A4CEEEE3-5EE5-4166-9A65-51E09840E49F}"/>
-    <hyperlink ref="G17" r:id="rId23" display="https://leetcode.com/problems/maximum-product-subarray/" xr:uid="{E66937F4-342E-466B-92BD-529EAD0F1180}"/>
-    <hyperlink ref="G18" r:id="rId24" display="https://leetcode.com/problems/maximum-length-of-subarray-with-positive-product/" xr:uid="{C0B6118F-C23A-4E55-881A-F4A1DA018A1F}"/>
+    <hyperlink ref="C62" r:id="rId19" xr:uid="{7FDCAB78-56F5-40D3-8A09-8A8A0E54E05D}"/>
+    <hyperlink ref="F63" r:id="rId20" xr:uid="{F7F3C873-8E94-4212-B22A-52BF75A478D8}"/>
+    <hyperlink ref="C28" r:id="rId21" xr:uid="{F6C15430-DBA9-4DAD-A411-65B1524C625E}"/>
+    <hyperlink ref="G17" r:id="rId22" display="https://leetcode.com/problems/maximum-sum-circular-subarray/" xr:uid="{A4CEEEE3-5EE5-4166-9A65-51E09840E49F}"/>
+    <hyperlink ref="G18" r:id="rId23" display="https://leetcode.com/problems/maximum-product-subarray/" xr:uid="{E66937F4-342E-466B-92BD-529EAD0F1180}"/>
+    <hyperlink ref="G19" r:id="rId24" display="https://leetcode.com/problems/maximum-length-of-subarray-with-positive-product/" xr:uid="{C0B6118F-C23A-4E55-881A-F4A1DA018A1F}"/>
     <hyperlink ref="C6" r:id="rId25" xr:uid="{D548A552-BEA3-46D9-89FD-0EDF330CCD4B}"/>
+    <hyperlink ref="C66" r:id="rId26" xr:uid="{7EAF2DCC-4594-46F5-AFC0-D19FF750F897}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId26"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId27"/>
   <headerFooter>
     <oddFooter>&amp;L12/30/2021&amp;CAXP Internal&amp;R1</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Binary Search and Divide and Conquer
</commit_message>
<xml_diff>
--- a/SDE Sheet.xlsx
+++ b/SDE Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Src Code\Personal\SDE-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F730376-E7E8-4480-80E5-361B39963BE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45FA4AC-2B2B-47E7-90A6-B715588F47FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83934561-A72F-4836-B1E7-4EE8C35F9874}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="269">
   <si>
     <t>Matrix</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>Graphs</t>
-  </si>
-  <si>
-    <t>Priority Queue</t>
   </si>
   <si>
     <t>Binary Search Tree</t>
@@ -927,6 +924,42 @@
   </si>
   <si>
     <t>Corner Cases and handle overflows/underflows</t>
+  </si>
+  <si>
+    <t>Read about Bidirectional BFS</t>
+  </si>
+  <si>
+    <t>Divide and Conquer</t>
+  </si>
+  <si>
+    <t>Inversion of Array</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/615?topList=striver-sde-sheet-problems&amp;utm_source=striver&amp;utm_medium=website</t>
+  </si>
+  <si>
+    <t>When greater element is at lesser index and sorted array helps indentify in O(n)</t>
+  </si>
+  <si>
+    <t>Read about Merge sort without extra space</t>
+  </si>
+  <si>
+    <t>Reverse Pairs</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-pairs/</t>
+  </si>
+  <si>
+    <t>Koko Eating Bananas</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/koko-eating-bananas/</t>
+  </si>
+  <si>
+    <t>O(n*log(m))</t>
+  </si>
+  <si>
+    <t>Try with Brute Force if nothing strikes and then convert to Binary Search</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1245,6 +1278,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1257,28 +1313,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1290,37 +1355,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1638,11 +1673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EBAEE5-B4E7-4BD5-B694-FD6EEA5E8AC0}">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="78" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="74" zoomScaleNormal="94" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1657,7 +1692,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>6</v>
@@ -1676,14 +1711,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
@@ -1723,43 +1758,43 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="41" t="s">
-        <v>36</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>14</v>
@@ -1774,10 +1809,10 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -1786,50 +1821,50 @@
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
@@ -1852,47 +1887,47 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1900,92 +1935,92 @@
         <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
       <c r="G20" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -2006,7 +2041,7 @@
         <v>27</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -2027,210 +2062,210 @@
         <v>27</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="G23" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="31"/>
       <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A26" s="30"/>
       <c r="B26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="32"/>
       <c r="B27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D27" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="30"/>
       <c r="B28" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="30"/>
       <c r="B29" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="51" t="s">
-        <v>241</v>
-      </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="53"/>
+      <c r="A30" s="63" t="s">
+        <v>240</v>
+      </c>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="65"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G31" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G31" s="38" t="s">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="38" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="38" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="G33" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="26"/>
       <c r="B34" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>18</v>
@@ -2242,16 +2277,16 @@
         <v>13</v>
       </c>
       <c r="G34" s="38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="26"/>
       <c r="B35" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>18</v>
@@ -2264,106 +2299,106 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="43"/>
-      <c r="B36" s="45" t="s">
+      <c r="A36" s="46"/>
+      <c r="B36" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="D36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="44"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="49"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
       <c r="B40" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="10"/>
       <c r="B41" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="59"/>
-      <c r="B42" s="39" t="s">
+      <c r="A42" s="53"/>
+      <c r="B42" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="50" t="s">
         <v>182</v>
-      </c>
-      <c r="C42" s="41" t="s">
-        <v>183</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>14</v>
@@ -2372,29 +2407,29 @@
         <v>4</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="54"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="60"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="54"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="60"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>18</v>
@@ -2404,27 +2439,27 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="61"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="42"/>
+      <c r="A45" s="55"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="51"/>
       <c r="D45" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="23"/>
       <c r="B46" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="C46" s="24" t="s">
-        <v>188</v>
-      </c>
       <c r="D46" s="2" t="s">
         <v>18</v>
       </c>
@@ -2432,53 +2467,53 @@
         <v>18</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="28"/>
       <c r="B47" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="C47" s="27" t="s">
+      <c r="D47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="28"/>
       <c r="B48" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="C48" s="27" t="s">
+      <c r="D48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="25"/>
       <c r="B49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C49" s="24" t="s">
-        <v>190</v>
-      </c>
       <c r="D49" s="2" t="s">
         <v>18</v>
       </c>
@@ -2486,7 +2521,7 @@
         <v>4</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2504,22 +2539,22 @@
         <v>4</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="9"/>
       <c r="B51" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>13</v>
@@ -2528,13 +2563,13 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="11"/>
       <c r="B52" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>4</v>
@@ -2544,116 +2579,116 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="46"/>
-      <c r="B53" s="39" t="s">
+      <c r="A53" s="59"/>
+      <c r="B53" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C53" s="41" t="s">
-        <v>234</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="60"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="64"/>
-      <c r="B54" s="62"/>
-      <c r="C54" s="63"/>
-      <c r="D54" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="60"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F55" s="37" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="64"/>
-      <c r="B55" s="62"/>
-      <c r="C55" s="63"/>
-      <c r="D55" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F55" s="37" t="s">
-        <v>239</v>
-      </c>
-    </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="64"/>
-      <c r="B56" s="62"/>
-      <c r="C56" s="63"/>
+      <c r="A56" s="60"/>
+      <c r="B56" s="56"/>
+      <c r="C56" s="57"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="64"/>
-      <c r="B57" s="62"/>
-      <c r="C57" s="63"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="57"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="64"/>
-      <c r="B58" s="62"/>
-      <c r="C58" s="63"/>
+      <c r="A58" s="60"/>
+      <c r="B58" s="56"/>
+      <c r="C58" s="57"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="47"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="42"/>
+      <c r="A59" s="61"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="51"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="B60" s="48"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
+      <c r="A60" s="58" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" s="58"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="58"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="58"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
       <c r="B61" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="54" t="s">
+      <c r="A62" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="55"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="56"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="45"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
@@ -2664,14 +2699,14 @@
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="48" t="s">
+      <c r="A64" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B64" s="48"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="48"/>
-      <c r="E64" s="48"/>
-      <c r="F64" s="48"/>
+      <c r="B64" s="58"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="58"/>
+      <c r="E64" s="58"/>
+      <c r="F64" s="58"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
@@ -2682,22 +2717,22 @@
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="48" t="s">
+      <c r="A66" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B66" s="48"/>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="58"/>
+      <c r="D66" s="58"/>
+      <c r="E66" s="58"/>
+      <c r="F66" s="58"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="11"/>
       <c r="B67" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>18</v>
@@ -2712,10 +2747,10 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="11"/>
       <c r="B68" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>18</v>
@@ -2728,47 +2763,47 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="50"/>
-      <c r="B69" s="45" t="s">
+      <c r="A69" s="66"/>
+      <c r="B69" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C69" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="C69" s="49" t="s">
+      <c r="D69" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="66"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="50"/>
-      <c r="B70" s="45"/>
-      <c r="C70" s="49"/>
-      <c r="D70" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="11"/>
       <c r="B71" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="D71" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>4</v>
@@ -2780,13 +2815,13 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="D72" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>4</v>
@@ -2798,193 +2833,193 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="11"/>
       <c r="B74" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="58"/>
-      <c r="B75" s="45" t="s">
+      <c r="A75" s="41"/>
+      <c r="B75" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C75" s="49" t="s">
-        <v>152</v>
-      </c>
       <c r="D75" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F75" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" s="41"/>
+      <c r="B76" s="52"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="58"/>
-      <c r="B76" s="45"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
     <row r="77" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="43"/>
-      <c r="B77" s="45" t="s">
+      <c r="A77" s="46"/>
+      <c r="B77" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C77" s="41" t="s">
+      <c r="D77" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D77" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F77" s="2" t="s">
+    </row>
+    <row r="78" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="47"/>
+      <c r="B78" s="52"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="44"/>
-      <c r="B78" s="45"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F78" s="1" t="s">
+    <row r="79" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="59"/>
+      <c r="B79" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="C79" s="50" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="46"/>
-      <c r="B79" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C79" s="41" t="s">
+      <c r="D79" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="61"/>
+      <c r="B80" s="52"/>
+      <c r="C80" s="51"/>
+      <c r="D80" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D79" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="47"/>
-      <c r="B80" s="45"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81" s="43"/>
-      <c r="B81" s="39" t="s">
+      <c r="A81" s="46"/>
+      <c r="B81" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="C81" s="41" t="s">
+      <c r="D81" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D81" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F81" s="2" t="s">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" s="47"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" s="44"/>
-      <c r="B82" s="40"/>
-      <c r="C82" s="42"/>
-      <c r="D82" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="22"/>
       <c r="B83" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C83" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="C83" s="20" t="s">
+      <c r="D83" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="E83" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="17"/>
       <c r="B84" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C84" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C84" s="15" t="s">
-        <v>161</v>
-      </c>
       <c r="D84" s="2" t="s">
         <v>18</v>
       </c>
@@ -2992,31 +3027,31 @@
         <v>4</v>
       </c>
       <c r="F84" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" s="62"/>
+      <c r="B85" s="52" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" s="57"/>
-      <c r="B85" s="45" t="s">
+      <c r="C85" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="C85" s="49" t="s">
+      <c r="D85" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="57"/>
-      <c r="B86" s="45"/>
-      <c r="C86" s="49"/>
+      <c r="A86" s="62"/>
+      <c r="B86" s="52"/>
+      <c r="C86" s="42"/>
       <c r="D86" s="2" t="s">
         <v>18</v>
       </c>
@@ -3024,26 +3059,26 @@
         <v>4</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="B87" s="48"/>
-      <c r="C87" s="48"/>
-      <c r="D87" s="48"/>
-      <c r="E87" s="48"/>
-      <c r="F87" s="48"/>
+      <c r="A87" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B87" s="58"/>
+      <c r="C87" s="58"/>
+      <c r="D87" s="58"/>
+      <c r="E87" s="58"/>
+      <c r="F87" s="58"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
-      <c r="B88" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C88" s="49" t="s">
-        <v>62</v>
+      <c r="B88" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C88" s="42" t="s">
+        <v>61</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>18</v>
@@ -3052,13 +3087,13 @@
         <v>18</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
-      <c r="B89" s="45"/>
-      <c r="C89" s="49"/>
+      <c r="B89" s="52"/>
+      <c r="C89" s="42"/>
       <c r="D89" s="2" t="s">
         <v>18</v>
       </c>
@@ -3066,31 +3101,31 @@
         <v>4</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
-      <c r="B90" s="45" t="s">
+      <c r="B90" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="C90" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C90" s="49" t="s">
+      <c r="D90" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
-      <c r="B91" s="45"/>
-      <c r="C91" s="49"/>
+      <c r="B91" s="52"/>
+      <c r="C91" s="42"/>
       <c r="D91" s="2" t="s">
         <v>18</v>
       </c>
@@ -3098,110 +3133,110 @@
         <v>4</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C92" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="D92" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C93" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="D93" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E93" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
-      <c r="B94" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C94" s="49" t="s">
+      <c r="B94" s="52" t="s">
         <v>83</v>
       </c>
+      <c r="C94" s="42" t="s">
+        <v>82</v>
+      </c>
       <c r="D94" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
-      <c r="B95" s="45"/>
-      <c r="C95" s="49"/>
+      <c r="B95" s="52"/>
+      <c r="C95" s="42"/>
       <c r="D95" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E95" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
-      <c r="B96" s="45" t="s">
+      <c r="B96" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C96" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C96" s="49" t="s">
-        <v>88</v>
-      </c>
       <c r="D96" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
-      <c r="B97" s="45"/>
-      <c r="C97" s="49"/>
+      <c r="B97" s="52"/>
+      <c r="C97" s="42"/>
       <c r="D97" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E97" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F97" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F97" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="14"/>
       <c r="C98" s="15"/>
@@ -3209,260 +3244,374 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A99" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="B99" s="48"/>
-      <c r="C99" s="48"/>
-      <c r="D99" s="48"/>
-      <c r="E99" s="48"/>
-      <c r="F99" s="48"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" s="58"/>
+      <c r="C99" s="58"/>
+      <c r="D99" s="58"/>
+      <c r="E99" s="58"/>
+      <c r="F99" s="58"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D100" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="E100" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F100" s="4"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F101" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F101" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A102" s="48" t="s">
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="B102" s="48"/>
-      <c r="C102" s="48"/>
-      <c r="D102" s="48"/>
-      <c r="E102" s="48"/>
-      <c r="F102" s="48"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B102" s="58"/>
+      <c r="C102" s="58"/>
+      <c r="D102" s="58"/>
+      <c r="E102" s="58"/>
+      <c r="F102" s="58"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
       <c r="B103" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="E103" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F103" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D104" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="10"/>
       <c r="B105" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D105" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A106" s="48" t="s">
+      <c r="G105" s="39" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="B106" s="58"/>
+      <c r="C106" s="58"/>
+      <c r="D106" s="58"/>
+      <c r="E106" s="58"/>
+      <c r="F106" s="58"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107" s="9"/>
+      <c r="B107" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="G107" s="39" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" s="10"/>
+      <c r="B108" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="G108" s="40"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A109" s="10"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="40"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A110" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B110" s="58"/>
+      <c r="C110" s="58"/>
+      <c r="D110" s="58"/>
+      <c r="E110" s="58"/>
+      <c r="F110" s="58"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A111" s="9"/>
+      <c r="B111" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G111" s="40"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A112" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B106" s="48"/>
-      <c r="C106" s="48"/>
-      <c r="D106" s="48"/>
-      <c r="E106" s="48"/>
-      <c r="F106" s="48"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A108" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B108" s="48"/>
-      <c r="C108" s="48"/>
-      <c r="D108" s="48"/>
-      <c r="E108" s="48"/>
-      <c r="F108" s="48"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A109" s="2"/>
-      <c r="B109" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C109" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A110" s="2"/>
-      <c r="B110" s="45"/>
-      <c r="C110" s="45"/>
-      <c r="D110" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A111" s="2"/>
-      <c r="B111" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A112" s="2"/>
-      <c r="B112" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="C112" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="B112" s="58"/>
+      <c r="C112" s="58"/>
+      <c r="D112" s="58"/>
+      <c r="E112" s="58"/>
+      <c r="F112" s="58"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="2"/>
-      <c r="B113" s="45"/>
-      <c r="C113" s="49"/>
+      <c r="B113" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C113" s="42" t="s">
+        <v>110</v>
+      </c>
       <c r="D113" s="2" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F113" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A114" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B114" s="48"/>
-      <c r="C114" s="48"/>
-      <c r="D114" s="48"/>
-      <c r="E114" s="48"/>
-      <c r="F114" s="48"/>
+      <c r="A114" s="2"/>
+      <c r="B114" s="52"/>
+      <c r="C114" s="52"/>
+      <c r="D114" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
+      <c r="B115" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" s="2"/>
+      <c r="B116" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="C116" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F117" s="34" t="s">
-        <v>154</v>
+      <c r="A117" s="2"/>
+      <c r="B117" s="52"/>
+      <c r="C117" s="42"/>
+      <c r="D117" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F117" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F118" s="34" t="s">
-        <v>218</v>
-      </c>
+      <c r="A118" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B118" s="58"/>
+      <c r="C118" s="58"/>
+      <c r="D118" s="58"/>
+      <c r="E118" s="58"/>
+      <c r="F118" s="58"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F119" s="34" t="s">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F121" s="34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F122" s="34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F123" s="34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F124" s="36" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F120" s="36" t="s">
-        <v>227</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="57">
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="A118:F118"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A99:F99"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="A106:F106"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A110:F110"/>
     <mergeCell ref="A75:A76"/>
     <mergeCell ref="C75:C76"/>
     <mergeCell ref="A62:F62"/>
@@ -3479,46 +3628,6 @@
     <mergeCell ref="B53:B59"/>
     <mergeCell ref="A53:A59"/>
     <mergeCell ref="C53:C59"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="A106:F106"/>
-    <mergeCell ref="A108:F108"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A114:F114"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="A99:F99"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="B79:B80"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{3FB3FA06-DE47-4C2D-AFD7-F5FC45E3D126}"/>
@@ -3534,9 +3643,9 @@
     <hyperlink ref="C100" r:id="rId11" xr:uid="{914A5C5A-20B3-4526-A460-020F9852AFDB}"/>
     <hyperlink ref="C101" r:id="rId12" xr:uid="{0B2D15B8-18BF-46A5-991E-6E53ADC95851}"/>
     <hyperlink ref="C33" r:id="rId13" xr:uid="{93A177B9-936F-4ED5-9F32-EB31F0D8F614}"/>
-    <hyperlink ref="C109" r:id="rId14" xr:uid="{9CD2E86C-B1BA-4CC3-9E52-ECA767380715}"/>
-    <hyperlink ref="C111" r:id="rId15" xr:uid="{30EBB8AD-10BE-47B9-BF85-DBCCCE948784}"/>
-    <hyperlink ref="F113" r:id="rId16" xr:uid="{080A2B1B-6640-47F1-9DAB-1F0914BD9938}"/>
+    <hyperlink ref="C113" r:id="rId14" xr:uid="{9CD2E86C-B1BA-4CC3-9E52-ECA767380715}"/>
+    <hyperlink ref="C115" r:id="rId15" xr:uid="{30EBB8AD-10BE-47B9-BF85-DBCCCE948784}"/>
+    <hyperlink ref="F117" r:id="rId16" xr:uid="{080A2B1B-6640-47F1-9DAB-1F0914BD9938}"/>
     <hyperlink ref="C67" r:id="rId17" xr:uid="{DD8AB0F8-5B5E-4F6E-A0B4-339B324BDAC3}"/>
     <hyperlink ref="C8" r:id="rId18" xr:uid="{43B67C49-DC70-412F-B095-E684E07FF196}"/>
     <hyperlink ref="C77" r:id="rId19" xr:uid="{7FDCAB78-56F5-40D3-8A09-8A8A0E54E05D}"/>
@@ -3553,9 +3662,10 @@
     <hyperlink ref="G33" r:id="rId30" display="https://leetcode.com/problems/meeting-rooms/" xr:uid="{8849EA4F-0A54-4D57-AE19-19728A56318A}"/>
     <hyperlink ref="G34" r:id="rId31" display="https://leetcode.com/problems/meeting-rooms-ii/" xr:uid="{DD819D71-EB3C-4BD3-BA6C-25223B20391D}"/>
     <hyperlink ref="C17" r:id="rId32" xr:uid="{6062919D-9F53-4AD6-A2BA-CE01278187C7}"/>
+    <hyperlink ref="C107" r:id="rId33" xr:uid="{7B7426B5-0217-46DE-ABCD-A2F2DDDDFB2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId33"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId34"/>
   <headerFooter>
     <oddFooter>&amp;L12/30/2021&amp;CAXP Internal&amp;R1</oddFooter>
   </headerFooter>

</xml_diff>